<commit_message>
compare branch of user
</commit_message>
<xml_diff>
--- a/assets/user.xlsx
+++ b/assets/user.xlsx
@@ -40,7 +40,7 @@
     <t>SINET</t>
   </si>
   <si>
-    <t>S.I GROUP HQ</t>
+    <t>S.I Group HQ</t>
   </si>
   <si>
     <t>SIN123457</t>
@@ -49,7 +49,7 @@
     <t>Sreynat</t>
   </si>
   <si>
-    <t>SINET SHN</t>
+    <t>S.I Group KPS</t>
   </si>
 </sst>
 </file>
@@ -436,7 +436,7 @@
   <cols>
     <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="19.433571428571426" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>

</xml_diff>